<commit_message>
data: updated list data of sources
</commit_message>
<xml_diff>
--- a/Data Files/LockdownEvents_Spreadsheet.xlsx
+++ b/Data Files/LockdownEvents_Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megancharles/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7e4705127bdb922/GitHub/WIDDatathon/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16071C0-5813-6348-8DCB-C8FBCA9E3D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A16071C0-5813-6348-8DCB-C8FBCA9E3D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{029F4445-3FEE-A941-B6B9-0117528FDE96}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6CB2CC52-2784-DB44-B5D6-BB8EFD7CB8FE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{6CB2CC52-2784-DB44-B5D6-BB8EFD7CB8FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>international-travel-covid.csv</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/grapher/covid-contact-tracing</t>
+  </si>
+  <si>
+    <t>https://github.com/geodatasource/country-borders</t>
   </si>
 </sst>
 </file>
@@ -275,28 +281,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -324,6 +308,28 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -338,14 +344,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{802EEE10-8A1C-164F-A70B-8724CFC064EA}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E11" xr:uid="{920F452F-E3D1-AE4F-BC99-B3581EFFA540}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{802EEE10-8A1C-164F-A70B-8724CFC064EA}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E13" xr:uid="{920F452F-E3D1-AE4F-BC99-B3581EFFA540}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9AAA2BAD-F141-DF4F-BB9E-EB457B5FEB84}" name="Lockdown event" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A6DDE828-A1D3-F248-B0DA-E355C49C7130}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{95CA21F2-58CA-7844-B87B-C46DCCBF8A34}" name="Link" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{66E37E21-CD8E-EC49-9874-748FB6F8ED56}" name="File name" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E8604EBF-B95C-C047-91EC-7B9BE9C6D307}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9AAA2BAD-F141-DF4F-BB9E-EB457B5FEB84}" name="Lockdown event" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A6DDE828-A1D3-F248-B0DA-E355C49C7130}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{95CA21F2-58CA-7844-B87B-C46DCCBF8A34}" name="Link" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{66E37E21-CD8E-EC49-9874-748FB6F8ED56}" name="File name" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E8604EBF-B95C-C047-91EC-7B9BE9C6D307}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BAD65D5-210E-1F42-A2C5-731D314230A7}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -824,6 +830,18 @@
         <v>45</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="data" display="https://www.bsg.ox.ac.uk/research/research-projects/coronavirus-government-response-tracker - data" xr:uid="{82798F85-AB41-9741-A738-56770E80D112}"/>
@@ -836,10 +854,12 @@
     <hyperlink ref="C9" r:id="rId8" xr:uid="{7BF9189A-3AF0-F54A-8B50-E245FA6A56F0}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{19451583-50F2-2747-B21E-0E34CE8D5E9C}"/>
     <hyperlink ref="C11" r:id="rId10" xr:uid="{2439DD13-BBFE-7C43-B1CB-3F0C48D28AA2}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{9597CA96-BE1F-D84D-9114-D06122F7AF00}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{604BCBA2-3E8F-3844-8802-9C04E5F99405}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>